<commit_message>
added links to lectures
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\source\repos\codingthematrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EBC9E2-6A13-47D2-838F-5ECAE7FCE3A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FF3ABE-35B9-4DF9-BEC7-C111D6DC9DBE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{4BCE7BA4-EBB2-4760-A29D-F5EEB46126C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4BCE7BA4-EBB2-4760-A29D-F5EEB46126C5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="coding_the_matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="d3_book" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>NumPagesPerDay</t>
   </si>
@@ -37,6 +38,87 @@
   </si>
   <si>
     <t>EndPage</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -390,10 +472,458 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC59359A-955B-4D14-8C9A-0120A9EE6449}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>513</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1">
+        <v>21</v>
+      </c>
+      <c r="M1">
+        <f>MOD(K1-$J$2,27)</f>
+        <v>18</v>
+      </c>
+      <c r="N1" t="str">
+        <f>VLOOKUP(M1,$P$1:$Q$27,2,FALSE)</f>
+        <v>s</v>
+      </c>
+      <c r="P1">
+        <v>0</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43498.490747800926</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43693</v>
+      </c>
+      <c r="C2">
+        <f>B2-A2</f>
+        <v>194.50925219907367</v>
+      </c>
+      <c r="F2" s="2">
+        <v>43498</v>
+      </c>
+      <c r="G2">
+        <v>41</v>
+      </c>
+      <c r="H2">
+        <v>45</v>
+      </c>
+      <c r="J2">
+        <v>30</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M11" si="0">MOD(K2-$J$2,27)</f>
+        <v>1</v>
+      </c>
+      <c r="N2" t="str">
+        <f t="shared" ref="N2:N11" si="1">VLOOKUP(M2,$P$1:$Q$27,2,FALSE)</f>
+        <v>b</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F3" s="2">
+        <v>43500</v>
+      </c>
+      <c r="G3">
+        <v>46</v>
+      </c>
+      <c r="H3">
+        <v>48</v>
+      </c>
+      <c r="K3">
+        <v>21</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" si="1"/>
+        <v>s</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F4" s="2">
+        <v>43501</v>
+      </c>
+      <c r="G4">
+        <v>49</v>
+      </c>
+      <c r="H4">
+        <v>51</v>
+      </c>
+      <c r="K4">
+        <v>11</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="1"/>
+        <v>i</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>43502</v>
+      </c>
+      <c r="G5">
+        <v>52</v>
+      </c>
+      <c r="H5">
+        <v>55</v>
+      </c>
+      <c r="K5">
+        <v>25</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="1"/>
+        <v>w</v>
+      </c>
+      <c r="P5">
+        <v>4</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f>A1/C2</f>
+        <v>2.6374066744905367</v>
+      </c>
+      <c r="F6" s="2">
+        <v>43503</v>
+      </c>
+      <c r="G6">
+        <v>56</v>
+      </c>
+      <c r="H6">
+        <v>58</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="1"/>
+        <v>a</v>
+      </c>
+      <c r="P6">
+        <v>5</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>11</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="1"/>
+        <v>i</v>
+      </c>
+      <c r="P7">
+        <v>6</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>21</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="1"/>
+        <v>s</v>
+      </c>
+      <c r="P8">
+        <v>7</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>(A1-H5)/C6</f>
+        <v>173.65543373718469</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="1"/>
+        <v>b</v>
+      </c>
+      <c r="P9">
+        <v>8</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f>A2+A9</f>
+        <v>43672.146181538112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>25</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="1"/>
+        <v>w</v>
+      </c>
+      <c r="P10">
+        <v>9</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>26</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="1"/>
+        <v>x</v>
+      </c>
+      <c r="P11">
+        <v>10</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <v>11</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <v>12</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>13</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <v>14</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>15</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>16</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <v>17</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>18</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <f>MOD(27,27)</f>
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>19</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <v>20</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <v>21</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="P23">
+        <v>22</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="P24">
+        <v>23</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="P25">
+        <v>24</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="P26">
+        <v>25</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="P27">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D7D276B-8435-47B6-B560-5BB1AB9711BF}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,7 +934,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>513</v>
+        <v>357</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -418,34 +948,56 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43498.490747800926</v>
+        <v>43502</v>
       </c>
       <c r="B2" s="2">
-        <v>43693</v>
+        <v>43585</v>
       </c>
       <c r="C2">
         <f>B2-A2</f>
-        <v>194.50925219907367</v>
+        <v>83</v>
       </c>
       <c r="F2" s="2">
-        <v>43498</v>
+        <v>43502</v>
       </c>
       <c r="G2">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>45</v>
-      </c>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>0</v>
       </c>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6">
         <f>A1/C2</f>
-        <v>2.6374066744905367</v>
+        <v>4.3012048192771086</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>(A1-H2)/C6</f>
+        <v>81.140056022408956</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f>A2+A9</f>
+        <v>43583.140056022406</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>